<commit_message>
Added data viewing func
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satya\PycharmProjects\99004340\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFFC1F6-32C6-49CE-8AF8-45710A1F64F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F05FA8-D6AB-4EA8-81E1-3B4BEB85B7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>PsNo</t>
   </si>
@@ -100,6 +101,123 @@
   </si>
   <si>
     <t>B+</t>
+  </si>
+  <si>
+    <t>Hobbie_1</t>
+  </si>
+  <si>
+    <t>Hobbie_2</t>
+  </si>
+  <si>
+    <t>Hobbie_3</t>
+  </si>
+  <si>
+    <t>Hobbie_4</t>
+  </si>
+  <si>
+    <t>Hobbie_5</t>
+  </si>
+  <si>
+    <t>Hobbie_6</t>
+  </si>
+  <si>
+    <t>Hobbie_7</t>
+  </si>
+  <si>
+    <t>Hobbie_8</t>
+  </si>
+  <si>
+    <t>Hobbie_9</t>
+  </si>
+  <si>
+    <t>Hobbie_10</t>
+  </si>
+  <si>
+    <t>Hobbie_11</t>
+  </si>
+  <si>
+    <t>Hobbie_12</t>
+  </si>
+  <si>
+    <t>Hobbie_13</t>
+  </si>
+  <si>
+    <t>Hobbie_14</t>
+  </si>
+  <si>
+    <t>Hobbie_15</t>
+  </si>
+  <si>
+    <t>Hobbie_16</t>
+  </si>
+  <si>
+    <t>Hobbie_17</t>
+  </si>
+  <si>
+    <t>Hobbie_18</t>
+  </si>
+  <si>
+    <t>Hobbie_19</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Skiing</t>
+  </si>
+  <si>
+    <t>Weight training</t>
+  </si>
+  <si>
+    <t>Postcard Collecting</t>
+  </si>
+  <si>
+    <t>Playing The Stock Market</t>
+  </si>
+  <si>
+    <t>Beekeeping</t>
+  </si>
+  <si>
+    <t>Playing Chess</t>
+  </si>
+  <si>
+    <t>Archery</t>
+  </si>
+  <si>
+    <t>Coin Collecting</t>
+  </si>
+  <si>
+    <t>Vintage Clothing Collecting</t>
+  </si>
+  <si>
+    <t>Furniture Building</t>
+  </si>
+  <si>
+    <t>LEGO</t>
+  </si>
+  <si>
+    <t>Amateur Radio</t>
+  </si>
+  <si>
+    <t>Sudoku</t>
+  </si>
+  <si>
+    <t>Crabbing</t>
+  </si>
+  <si>
+    <t>Kayaking</t>
+  </si>
+  <si>
+    <t>Parkour</t>
+  </si>
+  <si>
+    <t>Stamp Collecting</t>
+  </si>
+  <si>
+    <t>Wood Carving</t>
+  </si>
+  <si>
+    <t>Discpline_Grade</t>
   </si>
 </sst>
 </file>
@@ -426,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -450,10 +568,11 @@
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
     <col min="17" max="17" width="16.85546875" customWidth="1"/>
     <col min="18" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +630,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>99004000</v>
       </c>
@@ -570,68 +692,71 @@
       <c r="S2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>99004001</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>99004002</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>99004003</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99004004</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99004005</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>99004006</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>99004007</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>99004008</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>99004009</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99004010</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99004011</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>99004012</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>99004013</v>
       </c>
@@ -640,4 +765,229 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE74A5A-740A-4A79-A426-D39BB9681268}">
+  <dimension ref="A1:T15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>99004000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>99004001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>99004002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>99004003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>99004004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>99004005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>99004006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>99004007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>99004008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>99004009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>99004010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99004011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>99004012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>99004013</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added output data funcionality
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satya\PycharmProjects\99004340\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F05FA8-D6AB-4EA8-81E1-3B4BEB85B7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727858BB-1F72-4D13-B25C-7B44F85BDEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>